<commit_message>
first version of use types
</commit_message>
<xml_diff>
--- a/remap_ville_plugin/mapping_USE_TYPE.xlsx
+++ b/remap_ville_plugin/mapping_USE_TYPE.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20370"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shanshan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darthoma\Documents\GitHub\cea-remap-ville-plugin\remap_ville_plugin\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB0EFFC-3783-440A-B658-0FA62A42927D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="997" firstSheet="4" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="997" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SURB_2060_BAU" sheetId="18" r:id="rId1"/>
@@ -112,7 +113,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -476,24 +477,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="29.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.41796875" customWidth="1"/>
+    <col min="2" max="2" width="17.26171875" customWidth="1"/>
+    <col min="3" max="3" width="17.578125" customWidth="1"/>
+    <col min="6" max="6" width="17.83984375" customWidth="1"/>
+    <col min="7" max="7" width="29.26171875" customWidth="1"/>
+    <col min="9" max="9" width="13.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -531,7 +532,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -569,7 +570,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -607,7 +608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -645,7 +646,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -689,24 +690,24 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="29.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.41796875" customWidth="1"/>
+    <col min="2" max="2" width="17.26171875" customWidth="1"/>
+    <col min="3" max="3" width="17.578125" customWidth="1"/>
+    <col min="6" max="6" width="17.83984375" customWidth="1"/>
+    <col min="7" max="7" width="29.26171875" customWidth="1"/>
+    <col min="9" max="9" width="13.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -744,7 +745,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -782,7 +783,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -820,7 +821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -858,7 +859,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -902,24 +903,24 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="29.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.41796875" customWidth="1"/>
+    <col min="2" max="2" width="17.26171875" customWidth="1"/>
+    <col min="3" max="3" width="17.578125" customWidth="1"/>
+    <col min="6" max="6" width="17.83984375" customWidth="1"/>
+    <col min="7" max="7" width="29.26171875" customWidth="1"/>
+    <col min="9" max="9" width="13.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -957,7 +958,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -995,7 +996,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1033,7 +1034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -1071,7 +1072,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -1115,24 +1116,24 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="29.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.41796875" customWidth="1"/>
+    <col min="2" max="2" width="17.26171875" customWidth="1"/>
+    <col min="3" max="3" width="17.578125" customWidth="1"/>
+    <col min="6" max="6" width="17.83984375" customWidth="1"/>
+    <col min="7" max="7" width="29.26171875" customWidth="1"/>
+    <col min="9" max="9" width="13.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1170,7 +1171,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1208,7 +1209,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1246,7 +1247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -1284,7 +1285,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -1328,24 +1329,24 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="29.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.41796875" customWidth="1"/>
+    <col min="2" max="2" width="17.26171875" customWidth="1"/>
+    <col min="3" max="3" width="17.578125" customWidth="1"/>
+    <col min="6" max="6" width="17.83984375" customWidth="1"/>
+    <col min="7" max="7" width="29.26171875" customWidth="1"/>
+    <col min="9" max="9" width="13.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1383,7 +1384,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1421,7 +1422,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1459,7 +1460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -1497,7 +1498,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -1541,24 +1542,24 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="29.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.41796875" customWidth="1"/>
+    <col min="2" max="2" width="17.26171875" customWidth="1"/>
+    <col min="3" max="3" width="17.578125" customWidth="1"/>
+    <col min="6" max="6" width="17.83984375" customWidth="1"/>
+    <col min="7" max="7" width="29.26171875" customWidth="1"/>
+    <col min="9" max="9" width="13.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1596,7 +1597,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1634,7 +1635,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1672,7 +1673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -1710,7 +1711,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -1754,24 +1755,24 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="29.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.41796875" customWidth="1"/>
+    <col min="2" max="2" width="17.26171875" customWidth="1"/>
+    <col min="3" max="3" width="17.578125" customWidth="1"/>
+    <col min="6" max="6" width="17.83984375" customWidth="1"/>
+    <col min="7" max="7" width="29.26171875" customWidth="1"/>
+    <col min="9" max="9" width="13.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1809,7 +1810,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1847,7 +1848,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1885,7 +1886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -1923,7 +1924,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -1967,24 +1968,24 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="29.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.41796875" customWidth="1"/>
+    <col min="2" max="2" width="17.26171875" customWidth="1"/>
+    <col min="3" max="3" width="17.578125" customWidth="1"/>
+    <col min="6" max="6" width="17.83984375" customWidth="1"/>
+    <col min="7" max="7" width="29.26171875" customWidth="1"/>
+    <col min="9" max="9" width="13.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2022,7 +2023,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2060,7 +2061,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -2098,7 +2099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -2136,7 +2137,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -2180,24 +2181,24 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="29.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.41796875" customWidth="1"/>
+    <col min="2" max="2" width="17.26171875" customWidth="1"/>
+    <col min="3" max="3" width="17.578125" customWidth="1"/>
+    <col min="6" max="6" width="17.83984375" customWidth="1"/>
+    <col min="7" max="7" width="29.26171875" customWidth="1"/>
+    <col min="9" max="9" width="13.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2235,7 +2236,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2273,7 +2274,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -2311,7 +2312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -2349,7 +2350,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -2393,24 +2394,24 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="29.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.41796875" customWidth="1"/>
+    <col min="2" max="2" width="17.26171875" customWidth="1"/>
+    <col min="3" max="3" width="17.578125" customWidth="1"/>
+    <col min="6" max="6" width="17.83984375" customWidth="1"/>
+    <col min="7" max="7" width="29.26171875" customWidth="1"/>
+    <col min="9" max="9" width="13.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2448,7 +2449,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2486,7 +2487,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -2524,7 +2525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -2562,7 +2563,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -2606,24 +2607,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="29.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.41796875" customWidth="1"/>
+    <col min="2" max="2" width="17.26171875" customWidth="1"/>
+    <col min="3" max="3" width="17.578125" customWidth="1"/>
+    <col min="6" max="6" width="17.83984375" customWidth="1"/>
+    <col min="7" max="7" width="29.26171875" customWidth="1"/>
+    <col min="9" max="9" width="13.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2661,7 +2662,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2699,7 +2700,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -2737,7 +2738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -2775,7 +2776,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -2819,24 +2820,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="29.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.41796875" customWidth="1"/>
+    <col min="2" max="2" width="17.26171875" customWidth="1"/>
+    <col min="3" max="3" width="17.578125" customWidth="1"/>
+    <col min="6" max="6" width="17.83984375" customWidth="1"/>
+    <col min="7" max="7" width="29.26171875" customWidth="1"/>
+    <col min="9" max="9" width="13.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2874,7 +2875,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -2912,7 +2913,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -2950,7 +2951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -2988,7 +2989,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -3032,24 +3033,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="29.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.41796875" customWidth="1"/>
+    <col min="2" max="2" width="17.26171875" customWidth="1"/>
+    <col min="3" max="3" width="17.578125" customWidth="1"/>
+    <col min="6" max="6" width="17.83984375" customWidth="1"/>
+    <col min="7" max="7" width="29.26171875" customWidth="1"/>
+    <col min="9" max="9" width="13.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3087,7 +3088,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -3125,7 +3126,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -3163,7 +3164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -3201,7 +3202,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -3245,24 +3246,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="29.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.41796875" customWidth="1"/>
+    <col min="2" max="2" width="17.26171875" customWidth="1"/>
+    <col min="3" max="3" width="17.578125" customWidth="1"/>
+    <col min="6" max="6" width="17.83984375" customWidth="1"/>
+    <col min="7" max="7" width="29.26171875" customWidth="1"/>
+    <col min="9" max="9" width="13.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3300,7 +3301,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -3338,7 +3339,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -3376,7 +3377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -3414,7 +3415,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -3458,24 +3459,24 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="29.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.41796875" customWidth="1"/>
+    <col min="2" max="2" width="17.26171875" customWidth="1"/>
+    <col min="3" max="3" width="17.578125" customWidth="1"/>
+    <col min="6" max="6" width="17.83984375" customWidth="1"/>
+    <col min="7" max="7" width="29.26171875" customWidth="1"/>
+    <col min="9" max="9" width="13.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3513,7 +3514,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -3551,7 +3552,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -3589,7 +3590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -3627,7 +3628,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -3671,24 +3672,24 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="29.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.41796875" customWidth="1"/>
+    <col min="2" max="2" width="17.26171875" customWidth="1"/>
+    <col min="3" max="3" width="17.578125" customWidth="1"/>
+    <col min="6" max="6" width="17.83984375" customWidth="1"/>
+    <col min="7" max="7" width="29.26171875" customWidth="1"/>
+    <col min="9" max="9" width="13.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3726,7 +3727,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -3764,7 +3765,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -3802,7 +3803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -3840,7 +3841,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -3884,24 +3885,237 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="16.41796875" customWidth="1"/>
+    <col min="2" max="2" width="17.26171875" customWidth="1"/>
+    <col min="3" max="3" width="17.578125" customWidth="1"/>
+    <col min="6" max="6" width="17.83984375" customWidth="1"/>
+    <col min="7" max="7" width="29.26171875" customWidth="1"/>
+    <col min="9" max="9" width="13.83984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="29.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.41796875" customWidth="1"/>
+    <col min="2" max="2" width="17.26171875" customWidth="1"/>
+    <col min="3" max="3" width="17.578125" customWidth="1"/>
+    <col min="6" max="6" width="17.83984375" customWidth="1"/>
+    <col min="7" max="7" width="29.26171875" customWidth="1"/>
+    <col min="9" max="9" width="13.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3939,7 +4153,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -3977,7 +4191,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -4015,7 +4229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -4053,220 +4267,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L5" s="4">
-        <v>0.2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="29.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" s="4">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="4">
-        <v>1</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="4">
-        <v>0</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="L4" s="4">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>

</xml_diff>